<commit_message>
with new docs to sort
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingTest/DocumentUnderstandingTest/Devis_societe_1.xlsx
+++ b/DocumentUnderstandingTest/DocumentUnderstandingTest/Devis_societe_1.xlsx
@@ -142,7 +142,7 @@
     <t xml:space="preserve">Siret : </t>
   </si>
   <si>
-    <t>123-456-789 1234</t>
+    <t>987-654-321 1234</t>
   </si>
 </sst>
 </file>
@@ -1706,8 +1706,8 @@
   </sheetPr>
   <dimension ref="B1:F30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView showGridLines="0" tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.765625" defaultRowHeight="26.15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1729,7 +1729,7 @@
       </c>
       <c r="F2" s="8">
         <f ca="1">TODAY()</f>
-        <v>43913</v>
+        <v>43914</v>
       </c>
     </row>
     <row r="3" spans="2:6" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.4">
@@ -1772,7 +1772,7 @@
       </c>
       <c r="F7" s="8">
         <f ca="1">F2+30</f>
-        <v>43943</v>
+        <v>43944</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="16" customHeight="1" x14ac:dyDescent="0.4">
@@ -1861,7 +1861,7 @@
     </row>
     <row r="17" spans="2:6" s="5" customFormat="1" ht="26.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="26">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>13</v>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="F17" s="22">
         <f>IFERROR(IF(OR(Tableau_Articles[[#This Row],[Quantité]]="",Tableau_Articles[[#This Row],[Prix unitaire]]=""),"",Tableau_Articles[[#This Row],[Quantité]]*Tableau_Articles[[#This Row],[Prix unitaire]]),"")</f>
-        <v>4471.04</v>
+        <v>4750.4799999999996</v>
       </c>
     </row>
     <row r="18" spans="2:6" s="5" customFormat="1" ht="26.15" customHeight="1" x14ac:dyDescent="0.4">
@@ -1934,7 +1934,7 @@
       </c>
       <c r="F23" s="23">
         <f>SUM(Tableau_Articles[Montant])</f>
-        <v>4471.04</v>
+        <v>4750.4799999999996</v>
       </c>
     </row>
     <row r="24" spans="2:6" s="4" customFormat="1" ht="26.15" customHeight="1" x14ac:dyDescent="0.4">
@@ -1981,7 +1981,7 @@
       </c>
       <c r="F27" s="25">
         <f ca="1">SUM(F23,F25,F26)</f>
-        <v>4471.04</v>
+        <v>4750.4799999999996</v>
       </c>
     </row>
     <row r="28" spans="2:6" s="4" customFormat="1" ht="26.15" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -2044,6 +2044,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DEEA25CC0A0AC24199CDC46C25B8B0BC" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cf6cf056b5324d160236e2ac13572175">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="6dc4bcd6-49db-4c07-9060-8acfc67cef9f" xmlns:ns3="fb0879af-3eba-417a-a55a-ffe6dcd6ca77" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="308e4927137fd5e63b6be1bd7725299e" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2263,27 +2272,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49B3B314-6F37-4B5B-91DC-91848E4E7F4B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="fb0879af-3eba-417a-a55a-ffe6dcd6ca77"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="6dc4bcd6-49db-4c07-9060-8acfc67cef9f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fb0879af-3eba-417a-a55a-ffe6dcd6ca77"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
@@ -2291,6 +2291,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE21DFDB-9131-4336-BB9A-5B7FFEA41F63}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B971255C-6284-478A-B532-189CCBCEB2CD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2308,12 +2316,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE21DFDB-9131-4336-BB9A-5B7FFEA41F63}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>